<commit_message>
Updated translation file, Swedish and Czech language
git-svn-id: https://plugins.svn.wordpress.org/redi-restaurant-reservation/trunk@1207872 b8457f37-d9ea-0310-8a92-e5e31aec5664
</commit_message>
<xml_diff>
--- a/lang/Other translation.xlsx
+++ b/lang/Other translation.xlsx
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="172" uniqueCount="165">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="212" uniqueCount="195">
   <si>
     <t>duplicate_reservation</t>
   </si>
@@ -519,13 +519,103 @@
   </si>
   <si>
     <t>{0} person(s)</t>
+  </si>
+  <si>
+    <t>addon_inactive</t>
+  </si>
+  <si>
+    <t>Addon not activated.</t>
+  </si>
+  <si>
+    <t>reservation_in_past_cant_be_approved</t>
+  </si>
+  <si>
+    <t>Reservation that is in the past can not be approved.</t>
+  </si>
+  <si>
+    <t>reservation_in_past_cant_be_rejected</t>
+  </si>
+  <si>
+    <t>Reservation that is in the past can not be rejected.</t>
+  </si>
+  <si>
+    <t>reservation_not_available_for_today</t>
+  </si>
+  <si>
+    <t>Reservation is not available for today. Please select another day.</t>
+  </si>
+  <si>
+    <t>reservation_state_cant_be_changed</t>
+  </si>
+  <si>
+    <t>Reservation state can not be changed.</t>
+  </si>
+  <si>
+    <t>reservation_system_misconfiguration</t>
+  </si>
+  <si>
+    <t>We cannot accept your reservation for the selected date. Unable to find any available time to for reservation.</t>
+  </si>
+  <si>
+    <t>validation_email</t>
+  </si>
+  <si>
+    <t>Email is not valid.</t>
+  </si>
+  <si>
+    <t>New reservation successfully created #{0:### ###}</t>
+  </si>
+  <si>
+    <t>New Reservation</t>
+  </si>
+  <si>
+    <t>NewReservationModel_Comments</t>
+  </si>
+  <si>
+    <t>NewReservationModel_Date</t>
+  </si>
+  <si>
+    <t>NewReservationModel_Duration</t>
+  </si>
+  <si>
+    <t>Duration</t>
+  </si>
+  <si>
+    <t>NewReservationModel_Email</t>
+  </si>
+  <si>
+    <t>Email</t>
+  </si>
+  <si>
+    <t>NewReservationModel_Hour</t>
+  </si>
+  <si>
+    <t>Hour</t>
+  </si>
+  <si>
+    <t>NewReservationModel_Minutes</t>
+  </si>
+  <si>
+    <t>Minutes</t>
+  </si>
+  <si>
+    <t>NewReservationModel_Name</t>
+  </si>
+  <si>
+    <t>NewReservationModel_PartySize</t>
+  </si>
+  <si>
+    <t>NewReservationModel_Phone</t>
+  </si>
+  <si>
+    <t>NewReservationModel_ReservationDate</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <fonts count="2" x14ac:knownFonts="1">
+  <fonts count="3" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -535,6 +625,14 @@
     </font>
     <font>
       <b/>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <charset val="204"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
       <sz val="11"/>
       <color theme="1"/>
       <name val="Calibri"/>
@@ -563,7 +661,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="4">
+  <cellXfs count="5">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
@@ -572,6 +670,7 @@
       <alignment vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -852,10 +951,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:C89"/>
+  <dimension ref="A1:C109"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection sqref="A1:C1"/>
+    <sheetView tabSelected="1" topLeftCell="A98" workbookViewId="0">
+      <selection activeCell="A119" sqref="A119"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -876,683 +975,844 @@
         <v>38</v>
       </c>
     </row>
-    <row r="2" spans="1:3" ht="30" x14ac:dyDescent="0.25">
-      <c r="A2" s="1" t="s">
-        <v>0</v>
-      </c>
-      <c r="B2" s="1" t="s">
-        <v>1</v>
-      </c>
+    <row r="2" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A2" s="4" t="s">
+        <v>165</v>
+      </c>
+      <c r="B2" s="4" t="s">
+        <v>166</v>
+      </c>
+      <c r="C2" s="3"/>
     </row>
     <row r="3" spans="1:3" ht="30" x14ac:dyDescent="0.25">
       <c r="A3" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B3" s="1" t="s">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="4" spans="1:3" ht="30" x14ac:dyDescent="0.25">
+      <c r="A4" s="1" t="s">
         <v>2</v>
       </c>
-      <c r="B3" s="1" t="s">
+      <c r="B4" s="1" t="s">
         <v>3</v>
       </c>
     </row>
-    <row r="4" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A4" s="1" t="s">
+    <row r="5" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A5" s="1" t="s">
         <v>4</v>
       </c>
-      <c r="B4" s="1" t="s">
+      <c r="B5" s="1" t="s">
         <v>5</v>
       </c>
     </row>
-    <row r="5" spans="1:3" ht="45" x14ac:dyDescent="0.25">
-      <c r="A5" s="1" t="s">
-        <v>6</v>
-      </c>
-      <c r="B5" s="1" t="s">
-        <v>7</v>
-      </c>
-    </row>
-    <row r="6" spans="1:3" ht="120" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:3" ht="30" x14ac:dyDescent="0.25">
       <c r="A6" s="1" t="s">
-        <v>8</v>
+        <v>167</v>
       </c>
       <c r="B6" s="1" t="s">
-        <v>9</v>
+        <v>168</v>
       </c>
     </row>
     <row r="7" spans="1:3" ht="30" x14ac:dyDescent="0.25">
       <c r="A7" s="1" t="s">
+        <v>169</v>
+      </c>
+      <c r="B7" s="1" t="s">
+        <v>170</v>
+      </c>
+    </row>
+    <row r="8" spans="1:3" ht="45" x14ac:dyDescent="0.25">
+      <c r="A8" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="B8" s="1" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="9" spans="1:3" ht="120" x14ac:dyDescent="0.25">
+      <c r="A9" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="B9" s="1" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="10" spans="1:3" ht="30" x14ac:dyDescent="0.25">
+      <c r="A10" s="1" t="s">
         <v>10</v>
       </c>
-      <c r="B7" s="1" t="s">
+      <c r="B10" s="1" t="s">
         <v>11</v>
       </c>
     </row>
-    <row r="8" spans="1:3" ht="75" x14ac:dyDescent="0.25">
-      <c r="A8" s="1" t="s">
+    <row r="11" spans="1:3" ht="75" x14ac:dyDescent="0.25">
+      <c r="A11" s="1" t="s">
         <v>12</v>
       </c>
-      <c r="B8" s="1" t="s">
+      <c r="B11" s="1" t="s">
         <v>13</v>
-      </c>
-    </row>
-    <row r="9" spans="1:3" ht="45" x14ac:dyDescent="0.25">
-      <c r="A9" s="1" t="s">
-        <v>14</v>
-      </c>
-      <c r="B9" s="1" t="s">
-        <v>15</v>
-      </c>
-    </row>
-    <row r="10" spans="1:3" ht="45" x14ac:dyDescent="0.25">
-      <c r="A10" s="1" t="s">
-        <v>16</v>
-      </c>
-      <c r="B10" s="1" t="s">
-        <v>17</v>
-      </c>
-    </row>
-    <row r="11" spans="1:3" ht="45" x14ac:dyDescent="0.25">
-      <c r="A11" s="1" t="s">
-        <v>18</v>
-      </c>
-      <c r="B11" s="1" t="s">
-        <v>19</v>
       </c>
     </row>
     <row r="12" spans="1:3" ht="45" x14ac:dyDescent="0.25">
       <c r="A12" s="1" t="s">
-        <v>20</v>
+        <v>14</v>
       </c>
       <c r="B12" s="1" t="s">
-        <v>21</v>
-      </c>
-    </row>
-    <row r="13" spans="1:3" ht="45" x14ac:dyDescent="0.25">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="13" spans="1:3" ht="30" x14ac:dyDescent="0.25">
       <c r="A13" s="1" t="s">
-        <v>22</v>
+        <v>171</v>
       </c>
       <c r="B13" s="1" t="s">
-        <v>23</v>
+        <v>172</v>
       </c>
     </row>
     <row r="14" spans="1:3" ht="45" x14ac:dyDescent="0.25">
       <c r="A14" s="1" t="s">
-        <v>24</v>
+        <v>16</v>
       </c>
       <c r="B14" s="1" t="s">
-        <v>25</v>
+        <v>17</v>
       </c>
     </row>
     <row r="15" spans="1:3" ht="45" x14ac:dyDescent="0.25">
       <c r="A15" s="1" t="s">
-        <v>26</v>
+        <v>18</v>
       </c>
       <c r="B15" s="1" t="s">
-        <v>27</v>
+        <v>19</v>
       </c>
     </row>
     <row r="16" spans="1:3" ht="45" x14ac:dyDescent="0.25">
       <c r="A16" s="1" t="s">
-        <v>28</v>
+        <v>20</v>
       </c>
       <c r="B16" s="1" t="s">
-        <v>29</v>
+        <v>21</v>
       </c>
     </row>
     <row r="17" spans="1:2" ht="45" x14ac:dyDescent="0.25">
       <c r="A17" s="1" t="s">
+        <v>22</v>
+      </c>
+      <c r="B17" s="1" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="18" spans="1:2" ht="45" x14ac:dyDescent="0.25">
+      <c r="A18" s="1" t="s">
+        <v>24</v>
+      </c>
+      <c r="B18" s="1" t="s">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="19" spans="1:2" ht="45" x14ac:dyDescent="0.25">
+      <c r="A19" s="1" t="s">
+        <v>26</v>
+      </c>
+      <c r="B19" s="1" t="s">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="20" spans="1:2" ht="45" x14ac:dyDescent="0.25">
+      <c r="A20" s="1" t="s">
+        <v>28</v>
+      </c>
+      <c r="B20" s="1" t="s">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="21" spans="1:2" ht="45" x14ac:dyDescent="0.25">
+      <c r="A21" s="1" t="s">
         <v>30</v>
       </c>
-      <c r="B17" s="1" t="s">
+      <c r="B21" s="1" t="s">
         <v>31</v>
-      </c>
-    </row>
-    <row r="18" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A18" s="1" t="s">
-        <v>32</v>
-      </c>
-      <c r="B18" s="1" t="s">
-        <v>33</v>
-      </c>
-    </row>
-    <row r="19" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A19" s="1" t="s">
-        <v>34</v>
-      </c>
-      <c r="B19" s="1" t="s">
-        <v>35</v>
-      </c>
-    </row>
-    <row r="21" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A21" s="1" t="s">
-        <v>39</v>
-      </c>
-      <c r="B21" s="1" t="s">
-        <v>40</v>
       </c>
     </row>
     <row r="22" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A22" s="1" t="s">
+        <v>32</v>
+      </c>
+      <c r="B22" s="1" t="s">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="23" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A23" s="1" t="s">
+        <v>173</v>
+      </c>
+      <c r="B23" s="1" t="s">
+        <v>174</v>
+      </c>
+    </row>
+    <row r="24" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A24" s="1" t="s">
+        <v>175</v>
+      </c>
+      <c r="B24" s="1" t="s">
+        <v>176</v>
+      </c>
+    </row>
+    <row r="25" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A25" s="1" t="s">
+        <v>34</v>
+      </c>
+      <c r="B25" s="1" t="s">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="27" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A27" s="1" t="s">
+        <v>39</v>
+      </c>
+      <c r="B27" s="1" t="s">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="28" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A28" s="1" t="s">
         <v>41</v>
       </c>
-      <c r="B22" s="1" t="s">
+      <c r="B28" s="1" t="s">
         <v>41</v>
       </c>
     </row>
-    <row r="23" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A23" s="2" t="s">
+    <row r="29" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A29" s="2" t="s">
         <v>90</v>
-      </c>
-    </row>
-    <row r="24" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A24" t="s">
-        <v>42</v>
-      </c>
-      <c r="B24" t="s">
-        <v>43</v>
-      </c>
-    </row>
-    <row r="25" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A25" t="s">
-        <v>44</v>
-      </c>
-      <c r="B25" t="s">
-        <v>45</v>
-      </c>
-    </row>
-    <row r="26" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A26" t="s">
-        <v>46</v>
-      </c>
-      <c r="B26" t="s">
-        <v>47</v>
-      </c>
-    </row>
-    <row r="27" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A27" t="s">
-        <v>48</v>
-      </c>
-      <c r="B27" t="s">
-        <v>49</v>
-      </c>
-    </row>
-    <row r="28" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A28" t="s">
-        <v>50</v>
-      </c>
-      <c r="B28" t="s">
-        <v>51</v>
-      </c>
-    </row>
-    <row r="29" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A29" t="s">
-        <v>52</v>
-      </c>
-      <c r="B29" t="s">
-        <v>53</v>
       </c>
     </row>
     <row r="30" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A30" t="s">
-        <v>54</v>
+        <v>42</v>
       </c>
       <c r="B30" t="s">
-        <v>55</v>
+        <v>43</v>
       </c>
     </row>
     <row r="31" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A31" t="s">
-        <v>56</v>
+        <v>44</v>
       </c>
       <c r="B31" t="s">
-        <v>57</v>
+        <v>45</v>
       </c>
     </row>
     <row r="32" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A32" t="s">
-        <v>58</v>
+        <v>46</v>
       </c>
       <c r="B32" t="s">
-        <v>59</v>
+        <v>47</v>
       </c>
     </row>
     <row r="33" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A33" t="s">
-        <v>60</v>
+        <v>48</v>
       </c>
       <c r="B33" t="s">
-        <v>61</v>
+        <v>49</v>
       </c>
     </row>
     <row r="34" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A34" t="s">
-        <v>62</v>
+        <v>50</v>
       </c>
       <c r="B34" t="s">
-        <v>63</v>
+        <v>51</v>
       </c>
     </row>
     <row r="35" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A35" t="s">
-        <v>64</v>
+        <v>52</v>
       </c>
       <c r="B35" t="s">
-        <v>65</v>
+        <v>53</v>
       </c>
     </row>
     <row r="36" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A36" t="s">
-        <v>66</v>
+        <v>54</v>
       </c>
       <c r="B36" t="s">
-        <v>67</v>
+        <v>55</v>
       </c>
     </row>
     <row r="37" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A37" t="s">
-        <v>68</v>
+        <v>56</v>
       </c>
       <c r="B37" t="s">
-        <v>69</v>
+        <v>57</v>
       </c>
     </row>
     <row r="38" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A38" t="s">
-        <v>70</v>
+        <v>58</v>
       </c>
       <c r="B38" t="s">
-        <v>71</v>
+        <v>59</v>
       </c>
     </row>
     <row r="39" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A39" t="s">
-        <v>72</v>
+        <v>60</v>
       </c>
       <c r="B39" t="s">
-        <v>73</v>
+        <v>61</v>
       </c>
     </row>
     <row r="40" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A40" t="s">
-        <v>74</v>
+        <v>62</v>
       </c>
       <c r="B40" t="s">
-        <v>75</v>
+        <v>63</v>
       </c>
     </row>
     <row r="41" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A41" t="s">
-        <v>76</v>
+        <v>64</v>
       </c>
       <c r="B41" t="s">
-        <v>77</v>
+        <v>65</v>
       </c>
     </row>
     <row r="42" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A42" t="s">
-        <v>78</v>
+        <v>66</v>
       </c>
       <c r="B42" t="s">
-        <v>79</v>
+        <v>67</v>
       </c>
     </row>
     <row r="43" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A43" t="s">
-        <v>80</v>
+        <v>68</v>
       </c>
       <c r="B43" t="s">
-        <v>81</v>
+        <v>69</v>
       </c>
     </row>
     <row r="44" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A44" t="s">
-        <v>82</v>
+        <v>70</v>
       </c>
       <c r="B44" t="s">
-        <v>83</v>
+        <v>71</v>
       </c>
     </row>
     <row r="45" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A45" t="s">
-        <v>84</v>
+        <v>72</v>
       </c>
       <c r="B45" t="s">
-        <v>85</v>
+        <v>73</v>
       </c>
     </row>
     <row r="46" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A46" t="s">
-        <v>86</v>
+        <v>74</v>
       </c>
       <c r="B46" t="s">
-        <v>87</v>
+        <v>75</v>
       </c>
     </row>
     <row r="47" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A47" t="s">
+        <v>76</v>
+      </c>
+      <c r="B47" t="s">
+        <v>77</v>
+      </c>
+    </row>
+    <row r="48" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A48" t="s">
+        <v>78</v>
+      </c>
+      <c r="B48" t="s">
+        <v>79</v>
+      </c>
+    </row>
+    <row r="49" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A49" t="s">
+        <v>80</v>
+      </c>
+      <c r="B49" t="s">
+        <v>81</v>
+      </c>
+    </row>
+    <row r="50" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A50" t="s">
+        <v>82</v>
+      </c>
+      <c r="B50" t="s">
+        <v>83</v>
+      </c>
+    </row>
+    <row r="51" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A51" t="s">
+        <v>84</v>
+      </c>
+      <c r="B51" t="s">
+        <v>85</v>
+      </c>
+    </row>
+    <row r="52" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A52" t="s">
+        <v>86</v>
+      </c>
+      <c r="B52" t="s">
+        <v>87</v>
+      </c>
+    </row>
+    <row r="53" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A53" t="s">
         <v>88</v>
       </c>
-      <c r="B47" t="s">
+      <c r="B53" t="s">
         <v>89</v>
       </c>
     </row>
-    <row r="48" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A48" s="3" t="s">
+    <row r="54" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A54" s="3" t="s">
         <v>91</v>
       </c>
     </row>
-    <row r="49" spans="1:2" ht="30" x14ac:dyDescent="0.25">
-      <c r="A49" s="1" t="s">
+    <row r="55" spans="1:2" ht="30" x14ac:dyDescent="0.25">
+      <c r="A55" s="1" t="s">
         <v>92</v>
       </c>
-      <c r="B49" s="1" t="s">
+      <c r="B55" s="1" t="s">
         <v>93</v>
       </c>
     </row>
-    <row r="50" spans="1:2" ht="30" x14ac:dyDescent="0.25">
-      <c r="A50" s="1" t="s">
+    <row r="56" spans="1:2" ht="30" x14ac:dyDescent="0.25">
+      <c r="A56" s="1" t="s">
         <v>94</v>
       </c>
-      <c r="B50" s="1" t="s">
+      <c r="B56" s="1" t="s">
         <v>95</v>
-      </c>
-    </row>
-    <row r="51" spans="1:2" ht="30" x14ac:dyDescent="0.25">
-      <c r="A51" s="1" t="s">
-        <v>96</v>
-      </c>
-      <c r="B51" s="1" t="s">
-        <v>97</v>
-      </c>
-    </row>
-    <row r="52" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A52" s="1" t="s">
-        <v>98</v>
-      </c>
-      <c r="B52" s="1" t="s">
-        <v>99</v>
-      </c>
-    </row>
-    <row r="53" spans="1:2" ht="30" x14ac:dyDescent="0.25">
-      <c r="A53" s="1" t="s">
-        <v>100</v>
-      </c>
-      <c r="B53" s="1" t="s">
-        <v>101</v>
-      </c>
-    </row>
-    <row r="54" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A54" s="1" t="s">
-        <v>102</v>
-      </c>
-      <c r="B54" s="1" t="s">
-        <v>103</v>
-      </c>
-    </row>
-    <row r="56" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A56" s="2" t="s">
-        <v>104</v>
       </c>
     </row>
     <row r="57" spans="1:2" ht="30" x14ac:dyDescent="0.25">
       <c r="A57" s="1" t="s">
-        <v>105</v>
+        <v>96</v>
       </c>
       <c r="B57" s="1" t="s">
-        <v>106</v>
+        <v>97</v>
       </c>
     </row>
     <row r="58" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A58" s="1" t="s">
-        <v>107</v>
+        <v>98</v>
       </c>
       <c r="B58" s="1" t="s">
-        <v>108</v>
-      </c>
-    </row>
-    <row r="59" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A59" t="s">
-        <v>109</v>
-      </c>
-      <c r="B59" t="s">
-        <v>110</v>
+        <v>99</v>
+      </c>
+    </row>
+    <row r="59" spans="1:2" ht="30" x14ac:dyDescent="0.25">
+      <c r="A59" s="1" t="s">
+        <v>100</v>
+      </c>
+      <c r="B59" s="1" t="s">
+        <v>101</v>
       </c>
     </row>
     <row r="60" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A60" s="1" t="s">
-        <v>111</v>
+        <v>102</v>
       </c>
       <c r="B60" s="1" t="s">
-        <v>112</v>
-      </c>
-    </row>
-    <row r="61" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A61" s="1" t="s">
-        <v>113</v>
-      </c>
-      <c r="B61" s="1" t="s">
-        <v>114</v>
+        <v>103</v>
       </c>
     </row>
     <row r="62" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A62" s="1" t="s">
-        <v>115</v>
-      </c>
-      <c r="B62" s="1" t="s">
-        <v>116</v>
-      </c>
-    </row>
-    <row r="63" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A62" s="2" t="s">
+        <v>104</v>
+      </c>
+    </row>
+    <row r="63" spans="1:2" ht="30" x14ac:dyDescent="0.25">
       <c r="A63" s="1" t="s">
-        <v>117</v>
+        <v>105</v>
       </c>
       <c r="B63" s="1" t="s">
-        <v>118</v>
+        <v>106</v>
       </c>
     </row>
     <row r="64" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A64" s="1" t="s">
-        <v>119</v>
+        <v>107</v>
       </c>
       <c r="B64" s="1" t="s">
-        <v>120</v>
+        <v>108</v>
       </c>
     </row>
     <row r="65" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A65" s="1" t="s">
-        <v>121</v>
+        <v>177</v>
       </c>
       <c r="B65" s="1" t="s">
-        <v>122</v>
-      </c>
-    </row>
-    <row r="66" spans="1:2" ht="30" x14ac:dyDescent="0.25">
-      <c r="A66" s="1" t="s">
-        <v>123</v>
-      </c>
-      <c r="B66" s="1" t="s">
-        <v>124</v>
+        <v>178</v>
+      </c>
+    </row>
+    <row r="66" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A66" t="s">
+        <v>109</v>
+      </c>
+      <c r="B66" t="s">
+        <v>110</v>
       </c>
     </row>
     <row r="67" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A67" s="1" t="s">
-        <v>125</v>
+        <v>181</v>
       </c>
       <c r="B67" s="1" t="s">
-        <v>126</v>
-      </c>
-    </row>
-    <row r="68" spans="1:2" ht="30" x14ac:dyDescent="0.25">
+        <v>55</v>
+      </c>
+    </row>
+    <row r="68" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A68" s="1" t="s">
-        <v>127</v>
+        <v>182</v>
       </c>
       <c r="B68" s="1" t="s">
-        <v>128</v>
-      </c>
-    </row>
-    <row r="69" spans="1:2" ht="60" x14ac:dyDescent="0.25">
+        <v>59</v>
+      </c>
+    </row>
+    <row r="69" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A69" s="1" t="s">
-        <v>129</v>
+        <v>183</v>
       </c>
       <c r="B69" s="1" t="s">
-        <v>130</v>
-      </c>
-    </row>
-    <row r="70" spans="1:2" ht="30" x14ac:dyDescent="0.25">
+        <v>184</v>
+      </c>
+    </row>
+    <row r="70" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A70" s="1" t="s">
-        <v>131</v>
+        <v>185</v>
       </c>
       <c r="B70" s="1" t="s">
-        <v>132</v>
-      </c>
-    </row>
-    <row r="71" spans="1:2" ht="45" x14ac:dyDescent="0.25">
+        <v>186</v>
+      </c>
+    </row>
+    <row r="71" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A71" s="1" t="s">
-        <v>133</v>
+        <v>187</v>
       </c>
       <c r="B71" s="1" t="s">
-        <v>134</v>
-      </c>
-    </row>
-    <row r="72" spans="1:2" ht="45" x14ac:dyDescent="0.25">
+        <v>188</v>
+      </c>
+    </row>
+    <row r="72" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A72" s="1" t="s">
-        <v>135</v>
+        <v>189</v>
       </c>
       <c r="B72" s="1" t="s">
-        <v>136</v>
+        <v>190</v>
       </c>
     </row>
     <row r="73" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A73" s="1" t="s">
-        <v>137</v>
+        <v>191</v>
       </c>
       <c r="B73" s="1" t="s">
-        <v>138</v>
+        <v>51</v>
       </c>
     </row>
     <row r="74" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A74" s="1" t="s">
-        <v>119</v>
+        <v>192</v>
       </c>
       <c r="B74" s="1" t="s">
-        <v>139</v>
+        <v>67</v>
       </c>
     </row>
     <row r="75" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A75" s="1" t="s">
+        <v>193</v>
+      </c>
+      <c r="B75" s="1" t="s">
+        <v>53</v>
+      </c>
+    </row>
+    <row r="76" spans="1:2" ht="30" x14ac:dyDescent="0.25">
+      <c r="A76" s="1" t="s">
+        <v>194</v>
+      </c>
+      <c r="B76" s="1" t="s">
+        <v>59</v>
+      </c>
+    </row>
+    <row r="77" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A77" s="1" t="s">
+        <v>111</v>
+      </c>
+      <c r="B77" s="1" t="s">
+        <v>112</v>
+      </c>
+    </row>
+    <row r="78" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A78" s="1" t="s">
+        <v>113</v>
+      </c>
+      <c r="B78" s="1" t="s">
+        <v>114</v>
+      </c>
+    </row>
+    <row r="79" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A79" s="1" t="s">
+        <v>115</v>
+      </c>
+      <c r="B79" s="1" t="s">
+        <v>116</v>
+      </c>
+    </row>
+    <row r="80" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A80" s="1" t="s">
+        <v>117</v>
+      </c>
+      <c r="B80" s="1" t="s">
+        <v>118</v>
+      </c>
+    </row>
+    <row r="81" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A81" s="1" t="s">
+        <v>119</v>
+      </c>
+      <c r="B81" s="1" t="s">
+        <v>120</v>
+      </c>
+    </row>
+    <row r="82" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A82" s="1" t="s">
+        <v>121</v>
+      </c>
+      <c r="B82" s="1" t="s">
+        <v>122</v>
+      </c>
+    </row>
+    <row r="83" spans="1:2" ht="30" x14ac:dyDescent="0.25">
+      <c r="A83" s="1" t="s">
+        <v>123</v>
+      </c>
+      <c r="B83" s="1" t="s">
+        <v>124</v>
+      </c>
+    </row>
+    <row r="84" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A84" s="1" t="s">
+        <v>125</v>
+      </c>
+      <c r="B84" s="1" t="s">
+        <v>126</v>
+      </c>
+    </row>
+    <row r="85" spans="1:2" ht="30" x14ac:dyDescent="0.25">
+      <c r="A85" s="1" t="s">
+        <v>127</v>
+      </c>
+      <c r="B85" s="1" t="s">
+        <v>128</v>
+      </c>
+    </row>
+    <row r="86" spans="1:2" ht="60" x14ac:dyDescent="0.25">
+      <c r="A86" s="1" t="s">
+        <v>129</v>
+      </c>
+      <c r="B86" s="1" t="s">
+        <v>130</v>
+      </c>
+    </row>
+    <row r="87" spans="1:2" ht="30" x14ac:dyDescent="0.25">
+      <c r="A87" s="1" t="s">
+        <v>131</v>
+      </c>
+      <c r="B87" s="1" t="s">
+        <v>132</v>
+      </c>
+    </row>
+    <row r="88" spans="1:2" ht="45" x14ac:dyDescent="0.25">
+      <c r="A88" s="1" t="s">
+        <v>133</v>
+      </c>
+      <c r="B88" s="1" t="s">
+        <v>134</v>
+      </c>
+    </row>
+    <row r="89" spans="1:2" ht="45" x14ac:dyDescent="0.25">
+      <c r="A89" s="1" t="s">
+        <v>135</v>
+      </c>
+      <c r="B89" s="1" t="s">
+        <v>136</v>
+      </c>
+    </row>
+    <row r="90" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A90" s="1" t="s">
+        <v>137</v>
+      </c>
+      <c r="B90" s="1" t="s">
+        <v>138</v>
+      </c>
+    </row>
+    <row r="91" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A91" s="1" t="s">
+        <v>119</v>
+      </c>
+      <c r="B91" s="1" t="s">
+        <v>139</v>
+      </c>
+    </row>
+    <row r="92" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A92" s="1" t="s">
         <v>140</v>
       </c>
-      <c r="B75" s="1" t="s">
+      <c r="B92" s="1" t="s">
         <v>141</v>
       </c>
     </row>
-    <row r="76" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A76" t="s">
+    <row r="93" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A93" t="s">
         <v>142</v>
       </c>
-      <c r="B76" t="s">
+      <c r="B93" t="s">
         <v>143</v>
       </c>
     </row>
-    <row r="77" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A77" t="s">
+    <row r="94" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A94" t="s">
         <v>113</v>
       </c>
-      <c r="B77" t="s">
+      <c r="B94" t="s">
         <v>114</v>
       </c>
     </row>
-    <row r="78" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A78" t="s">
+    <row r="95" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A95" t="s">
         <v>144</v>
       </c>
-      <c r="B78" t="s">
+      <c r="B95" t="s">
         <v>145</v>
       </c>
     </row>
-    <row r="79" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A79" t="s">
+    <row r="96" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A96" t="s">
         <v>146</v>
       </c>
-      <c r="B79" t="s">
+      <c r="B96" t="s">
         <v>146</v>
       </c>
     </row>
-    <row r="80" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A80" t="s">
+    <row r="97" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A97" t="s">
         <v>147</v>
       </c>
-      <c r="B80" t="s">
+      <c r="B97" t="s">
         <v>148</v>
       </c>
     </row>
-    <row r="81" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A81" t="s">
+    <row r="98" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A98" t="s">
         <v>149</v>
       </c>
-      <c r="B81" t="s">
+      <c r="B98" t="s">
         <v>150</v>
       </c>
     </row>
-    <row r="82" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A82" t="s">
+    <row r="99" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A99" t="s">
         <v>151</v>
       </c>
-      <c r="B82" t="s">
+      <c r="B99" t="s">
         <v>152</v>
       </c>
     </row>
-    <row r="83" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A83" t="s">
+    <row r="100" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A100" t="s">
         <v>153</v>
       </c>
-      <c r="B83" t="s">
+      <c r="B100" t="s">
         <v>154</v>
       </c>
     </row>
-    <row r="84" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A84" t="s">
+    <row r="101" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A101" t="s">
         <v>155</v>
       </c>
-      <c r="B84" t="s">
+      <c r="B101" t="s">
         <v>156</v>
       </c>
     </row>
-    <row r="85" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A85" t="s">
+    <row r="102" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A102" t="s">
         <v>157</v>
       </c>
-      <c r="B85" t="s">
+      <c r="B102" t="s">
         <v>158</v>
       </c>
     </row>
-    <row r="86" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A86" t="s">
+    <row r="103" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A103" t="s">
         <v>159</v>
       </c>
-      <c r="B86" t="s">
+      <c r="B103" t="s">
         <v>160</v>
       </c>
     </row>
-    <row r="87" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A87" t="s">
+    <row r="104" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A104" t="s">
         <v>161</v>
       </c>
-      <c r="B87" t="s">
+      <c r="B104" t="s">
         <v>162</v>
       </c>
     </row>
-    <row r="88" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A88" t="s">
+    <row r="105" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A105" t="s">
         <v>163</v>
       </c>
-      <c r="B88" t="s">
+      <c r="B105" t="s">
         <v>164</v>
       </c>
     </row>
-    <row r="89" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A89" t="s">
+    <row r="106" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A106" t="s">
         <v>119</v>
       </c>
-      <c r="B89" t="s">
+      <c r="B106" t="s">
         <v>139</v>
+      </c>
+    </row>
+    <row r="107" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A107" s="1" t="s">
+        <v>113</v>
+      </c>
+      <c r="B107" s="1" t="s">
+        <v>114</v>
+      </c>
+    </row>
+    <row r="108" spans="1:2" ht="30" x14ac:dyDescent="0.25">
+      <c r="A108" s="1" t="s">
+        <v>115</v>
+      </c>
+      <c r="B108" s="1" t="s">
+        <v>179</v>
+      </c>
+    </row>
+    <row r="109" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A109" s="1" t="s">
+        <v>119</v>
+      </c>
+      <c r="B109" s="1" t="s">
+        <v>180</v>
       </c>
     </row>
   </sheetData>

</xml_diff>